<commit_message>
Added data provider and reporting
</commit_message>
<xml_diff>
--- a/src/main/java/resources/DataTest.xlsx
+++ b/src/main/java/resources/DataTest.xlsx
@@ -1,17 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{928D1546-64BE-4F13-B29C-54C5403AFFC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anuj\Selenium_Utilities\TutorialsNinja_Automation_Framework\src\main\java\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F2780DF-801B-44F5-BFE0-1D6C723187E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17304" windowHeight="12312" xr2:uid="{992C7C6A-9471-4AED-98A2-A3D1D2397718}"/>
+    <workbookView xWindow="2688" yWindow="1572" windowWidth="17280" windowHeight="8964" xr2:uid="{992C7C6A-9471-4AED-98A2-A3D1D2397718}"/>
   </bookViews>
   <sheets>
-    <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="userRegistration" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,22 +25,66 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>ankur</t>
-  </si>
-  <si>
-    <t>aman</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>confirmPwd</t>
+  </si>
+  <si>
+    <t>Prem</t>
+  </si>
+  <si>
+    <t>Mishra</t>
+  </si>
+  <si>
+    <t>Prem@gmail.com</t>
+  </si>
+  <si>
+    <t>prem123</t>
+  </si>
+  <si>
+    <t>Rajan</t>
+  </si>
+  <si>
+    <t>Sharma</t>
+  </si>
+  <si>
+    <t>Rajan@gmail.com</t>
+  </si>
+  <si>
+    <t>rajan123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -59,13 +107,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -378,23 +429,87 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F258FAD-4A95-4351-A79C-EBE9DE13998C}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" customWidth="1"/>
+    <col min="3" max="3" width="19.88671875" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2">
+        <v>2234456567</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>9678765321</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{E77F67A4-A3CE-4366-86E5-B73F85F073D5}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{CBDA698C-AEAA-4A4D-B67C-7F5A79DF2807}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added screenshots for failed test
</commit_message>
<xml_diff>
--- a/src/main/java/resources/DataTest.xlsx
+++ b/src/main/java/resources/DataTest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anuj\Selenium_Utilities\TutorialsNinja_Automation_Framework\src\main\java\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F2780DF-801B-44F5-BFE0-1D6C723187E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D17E4DD-CE78-49EA-8BF2-F2C9FD4E922F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="1572" windowWidth="17280" windowHeight="8964" xr2:uid="{992C7C6A-9471-4AED-98A2-A3D1D2397718}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{992C7C6A-9471-4AED-98A2-A3D1D2397718}"/>
   </bookViews>
   <sheets>
     <sheet name="userRegistration" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>firstName</t>
   </si>
@@ -57,16 +57,13 @@
     <t>prem123</t>
   </si>
   <si>
-    <t>Rajan</t>
-  </si>
-  <si>
-    <t>Sharma</t>
-  </si>
-  <si>
-    <t>Rajan@gmail.com</t>
-  </si>
-  <si>
-    <t>rajan123</t>
+    <t>Raman</t>
+  </si>
+  <si>
+    <t>Ram123ranm@gmail.com</t>
+  </si>
+  <si>
+    <t>raman123</t>
   </si>
 </sst>
 </file>
@@ -432,14 +429,14 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.6640625" customWidth="1"/>
     <col min="2" max="2" width="14.44140625" customWidth="1"/>
-    <col min="3" max="3" width="19.88671875" customWidth="1"/>
+    <col min="3" max="3" width="24.44140625" customWidth="1"/>
     <col min="4" max="4" width="12.5546875" customWidth="1"/>
     <col min="5" max="5" width="16.44140625" customWidth="1"/>
     <col min="6" max="6" width="16.6640625" customWidth="1"/>
@@ -490,25 +487,25 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3">
+        <v>352456565</v>
+      </c>
+      <c r="E3" t="s">
         <v>12</v>
       </c>
-      <c r="D3">
-        <v>9678765321</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{E77F67A4-A3CE-4366-86E5-B73F85F073D5}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{CBDA698C-AEAA-4A4D-B67C-7F5A79DF2807}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{FF91279A-84BF-480C-9886-4E39B4349BC7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added wishlist test cases
</commit_message>
<xml_diff>
--- a/src/main/java/resources/DataTest.xlsx
+++ b/src/main/java/resources/DataTest.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anuj\Selenium_Utilities\TutorialsNinja_Automation_Framework\src\main\java\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D17E4DD-CE78-49EA-8BF2-F2C9FD4E922F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{230133C1-48B0-43D6-8B07-27A46CE79CDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{992C7C6A-9471-4AED-98A2-A3D1D2397718}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{992C7C6A-9471-4AED-98A2-A3D1D2397718}"/>
   </bookViews>
   <sheets>
     <sheet name="userRegistration" sheetId="1" r:id="rId1"/>
+    <sheet name="MyAccountTable" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>firstName</t>
   </si>
@@ -64,6 +65,48 @@
   </si>
   <si>
     <t>raman123</t>
+  </si>
+  <si>
+    <t>Edit Account</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Address Book</t>
+  </si>
+  <si>
+    <t>Wish List</t>
+  </si>
+  <si>
+    <t>Order History</t>
+  </si>
+  <si>
+    <t>Downloads</t>
+  </si>
+  <si>
+    <t>Recurring payments</t>
+  </si>
+  <si>
+    <t>Reward Points</t>
+  </si>
+  <si>
+    <t>Returns</t>
+  </si>
+  <si>
+    <t>Transactions</t>
+  </si>
+  <si>
+    <t>Newsletter</t>
+  </si>
+  <si>
+    <t>Logout</t>
+  </si>
+  <si>
+    <t>My Account</t>
+  </si>
+  <si>
+    <t>Data</t>
   </si>
 </sst>
 </file>
@@ -428,7 +471,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F258FAD-4A95-4351-A79C-EBE9DE13998C}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -509,4 +552,93 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{679BF7BB-AC51-4A5E-BA67-74DB76A47A6C}">
+  <dimension ref="A1:A14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>